<commit_message>
update to fixing files (from a long time ago)
</commit_message>
<xml_diff>
--- a/src/zika_compilation/zika_db1_qa_fixing.xlsx
+++ b/src/zika_compilation/zika_db1_qa_fixing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/kem22_ic_ac_uk/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wpia-didef4.dide.ic.ac.uk\prioritypathogens\Zika\priority-pathogens\src\zika_compilation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="213" documentId="8_{0DCE3716-0B1F-4B7B-A721-7BCDFE8AAC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{338D9EAF-2C9D-4F02-85CE-9B11BA4BF6B7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605CB851-946A-4E4E-990D-0E83FEA0AB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="qa_fixing" sheetId="1" r:id="rId1"/>
@@ -421,7 +421,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -604,6 +604,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -768,7 +774,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -776,6 +782,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1153,17 +1160,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1204,7 +1211,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1245,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1286,7 +1293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1327,7 +1334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1368,7 +1375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1409,7 +1416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1450,7 +1457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1491,7 +1498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1532,7 +1539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1573,7 +1580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1614,7 +1621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1655,7 +1662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1696,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1737,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1778,7 +1785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1819,7 +1826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1860,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1901,7 +1908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1942,7 +1949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1983,7 +1990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2024,7 +2031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2065,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2106,7 +2113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2147,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2188,7 +2195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2229,7 +2236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2270,7 +2277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2311,7 +2318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2352,7 +2359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1</v>
       </c>
@@ -2393,7 +2400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2434,7 +2441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2475,7 +2482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2516,7 +2523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1</v>
       </c>
@@ -2557,7 +2564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1</v>
       </c>
@@ -2598,48 +2605,48 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>1</v>
-      </c>
-      <c r="B36">
+    <row r="36" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="5">
+        <v>1</v>
+      </c>
+      <c r="B36" s="5">
         <v>1496</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E36" t="s">
-        <v>15</v>
-      </c>
-      <c r="F36" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" t="s">
-        <v>15</v>
-      </c>
-      <c r="H36" t="s">
-        <v>15</v>
-      </c>
-      <c r="I36" t="s">
-        <v>15</v>
-      </c>
-      <c r="J36" t="s">
-        <v>15</v>
-      </c>
-      <c r="K36" t="s">
-        <v>15</v>
-      </c>
-      <c r="L36">
-        <v>1</v>
-      </c>
-      <c r="M36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E36" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="5">
+        <v>1</v>
+      </c>
+      <c r="M36" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1</v>
       </c>
@@ -2680,7 +2687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1</v>
       </c>
@@ -2721,7 +2728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1</v>
       </c>
@@ -2762,7 +2769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1</v>
       </c>
@@ -2803,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1</v>
       </c>
@@ -2844,7 +2851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>1</v>
       </c>
@@ -2885,7 +2892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>1</v>
       </c>
@@ -2926,7 +2933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1</v>
       </c>
@@ -2967,7 +2974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>1</v>
       </c>
@@ -3008,7 +3015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>1</v>
       </c>

</xml_diff>